<commit_message>
script to model average different corhmm models and demonstrates that Mk models can be converted into HMMs by duplicating them as multiple rate classes
</commit_message>
<xml_diff>
--- a/table_corhmm/SummaryTable_corHMM.xlsx
+++ b/table_corhmm/SummaryTable_corHMM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesboyko/2021_SeedDispersal/table_corhmm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1F45DC-68BE-DB42-AA0F-6AF83A2A5CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5A6441-5321-2847-A010-C5649CE6E24D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="820" windowWidth="28800" windowHeight="16120" xr2:uid="{E8FAF0D3-A3C2-C441-AEDE-9CF197D671DA}"/>
+    <workbookView xWindow="580" yWindow="-19540" windowWidth="28800" windowHeight="16120" xr2:uid="{E8FAF0D3-A3C2-C441-AEDE-9CF197D671DA}"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="60">
   <si>
     <t>k.rate</t>
   </si>
@@ -582,7 +582,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,9 +591,7 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="I1" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -720,7 +718,7 @@
   <dimension ref="A1:P446"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1158,7 +1156,7 @@
         <v>28</v>
       </c>
       <c r="N14">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="O14">
         <v>5.7000000000000002E-2</v>
@@ -1178,7 +1176,7 @@
         <v>26</v>
       </c>
       <c r="M15">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="N15" t="s">
         <v>28</v>
@@ -5173,7 +5171,7 @@
   <dimension ref="A1:P1718"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19799,7 +19797,7 @@
   <dimension ref="A1:P1240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30600,7 +30598,7 @@
   <dimension ref="A1:P1022"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>